<commit_message>
CS0902: Ajuste de publicación en GRECO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion02/EsqueletoGuion_CS_09_02_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion02/EsqueletoGuion_CS_09_02_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9258" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,20 +18,20 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="79">
   <si>
     <t>FICHA</t>
   </si>
@@ -187,9 +192,6 @@
     <t xml:space="preserve">La Italia fascista </t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje:  La Italia fascista</t>
-  </si>
-  <si>
     <t>La década de 1930</t>
   </si>
   <si>
@@ -259,16 +261,13 @@
     <t>Autoevaluación</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: los felices años veinte</t>
-  </si>
-  <si>
     <t>Distingue las características del fascismo</t>
   </si>
   <si>
     <t>Cronología: el período de entreguerras</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje:  la Italia fascista</t>
+    <t>Los felices años 20</t>
   </si>
 </sst>
 </file>
@@ -1696,7 +1695,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1706,41 +1705,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -1748,7 +1747,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1756,7 +1755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
@@ -1780,22 +1779,22 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E15" sqref="A15:E15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1815,7 +1814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="57" t="s">
         <v>31</v>
       </c>
@@ -1823,13 +1822,13 @@
         <v>19</v>
       </c>
       <c r="C2" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="57" t="s">
         <v>66</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>67</v>
       </c>
       <c r="F2" s="17">
         <v>1</v>
@@ -1841,7 +1840,7 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="57" t="s">
         <v>31</v>
       </c>
@@ -1849,19 +1848,19 @@
         <v>19</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="57" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="57" t="s">
         <v>31</v>
       </c>
@@ -1869,19 +1868,19 @@
         <v>19</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="57" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F4" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="57" t="s">
         <v>31</v>
       </c>
@@ -1889,19 +1888,19 @@
         <v>19</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="57" t="s">
         <v>49</v>
       </c>
       <c r="E5" s="57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F5" s="17">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="57" t="s">
         <v>31</v>
       </c>
@@ -1909,19 +1908,19 @@
         <v>19</v>
       </c>
       <c r="C6" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="57" t="s">
         <v>66</v>
-      </c>
-      <c r="D6" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="57" t="s">
-        <v>67</v>
       </c>
       <c r="F6" s="17">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="59" t="s">
         <v>31</v>
       </c>
@@ -1929,19 +1928,19 @@
         <v>19</v>
       </c>
       <c r="C7" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="59" t="s">
         <v>66</v>
-      </c>
-      <c r="D7" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="59" t="s">
-        <v>67</v>
       </c>
       <c r="F7" s="17">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="57" t="s">
         <v>31</v>
       </c>
@@ -1949,19 +1948,19 @@
         <v>19</v>
       </c>
       <c r="C8" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="57" t="s">
         <v>66</v>
-      </c>
-      <c r="D8" s="57" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="57" t="s">
-        <v>67</v>
       </c>
       <c r="F8" s="17">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="59" t="s">
         <v>31</v>
       </c>
@@ -1969,20 +1968,20 @@
         <v>19</v>
       </c>
       <c r="C9" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="59" t="s">
         <v>66</v>
-      </c>
-      <c r="D9" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="59" t="s">
-        <v>67</v>
       </c>
       <c r="F9" s="17">
         <v>8</v>
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="57" t="s">
         <v>31</v>
       </c>
@@ -1990,20 +1989,20 @@
         <v>19</v>
       </c>
       <c r="C10" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="57" t="s">
         <v>66</v>
-      </c>
-      <c r="D10" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="57" t="s">
-        <v>67</v>
       </c>
       <c r="F10" s="17">
         <v>9</v>
       </c>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="57" t="s">
         <v>31</v>
       </c>
@@ -2011,20 +2010,20 @@
         <v>19</v>
       </c>
       <c r="C11" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="57" t="s">
         <v>66</v>
-      </c>
-      <c r="D11" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="57" t="s">
-        <v>67</v>
       </c>
       <c r="F11" s="17">
         <v>10</v>
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="57" t="s">
         <v>31</v>
       </c>
@@ -2032,20 +2031,20 @@
         <v>19</v>
       </c>
       <c r="C12" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="57" t="s">
         <v>66</v>
-      </c>
-      <c r="D12" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="57" t="s">
-        <v>67</v>
       </c>
       <c r="F12" s="17">
         <v>11</v>
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="57" t="s">
         <v>31</v>
       </c>
@@ -2053,19 +2052,19 @@
         <v>19</v>
       </c>
       <c r="C13" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="57" t="s">
         <v>66</v>
-      </c>
-      <c r="D13" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="57" t="s">
-        <v>67</v>
       </c>
       <c r="F13" s="17">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="57" t="s">
         <v>31</v>
       </c>
@@ -2073,19 +2072,19 @@
         <v>19</v>
       </c>
       <c r="C14" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="57" t="s">
         <v>66</v>
-      </c>
-      <c r="D14" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="57" t="s">
-        <v>67</v>
       </c>
       <c r="F14" s="17">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="59" t="s">
         <v>31</v>
       </c>
@@ -2093,19 +2092,19 @@
         <v>19</v>
       </c>
       <c r="C15" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="59" t="s">
         <v>66</v>
-      </c>
-      <c r="D15" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="59" t="s">
-        <v>67</v>
       </c>
       <c r="F15" s="17">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="57" t="s">
         <v>31</v>
       </c>
@@ -2113,19 +2112,19 @@
         <v>19</v>
       </c>
       <c r="C16" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="57" t="s">
         <v>66</v>
-      </c>
-      <c r="D16" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="57" t="s">
-        <v>67</v>
       </c>
       <c r="F16" s="17">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="57" t="s">
         <v>31</v>
       </c>
@@ -2133,19 +2132,19 @@
         <v>19</v>
       </c>
       <c r="C17" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="57" t="s">
         <v>66</v>
-      </c>
-      <c r="D17" s="57" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="57" t="s">
-        <v>67</v>
       </c>
       <c r="F17" s="17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="57" t="s">
         <v>31</v>
       </c>
@@ -2153,13 +2152,13 @@
         <v>19</v>
       </c>
       <c r="C18" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="57" t="s">
         <v>66</v>
-      </c>
-      <c r="D18" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="57" t="s">
-        <v>67</v>
       </c>
       <c r="F18" s="17">
         <v>17</v>
@@ -2184,13 +2183,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -2201,9 +2200,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>21</v>
@@ -2212,9 +2211,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>21</v>
@@ -2223,7 +2222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>22</v>
       </c>
@@ -2234,9 +2233,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>21</v>
@@ -2245,12 +2244,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="56"/>
       <c r="B6" s="56"/>
       <c r="C6" s="56"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="56"/>
       <c r="B7" s="56"/>
       <c r="C7" s="56"/>
@@ -2271,7 +2270,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D37"/>
@@ -2280,14 +2279,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -2298,18 +2297,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -2320,7 +2319,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -2331,7 +2330,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -2342,18 +2341,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="14">
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -2364,151 +2363,151 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="14">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="14">
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="14">
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="14">
         <v>10</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="14">
         <v>11</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="14">
         <v>12</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="31"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="14">
         <v>13</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="14">
         <v>14</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="14">
         <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="14">
         <v>16</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="14">
         <v>17</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="14">
         <v>18</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="14">
         <v>19</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -2519,7 +2518,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -2530,77 +2529,77 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="27"/>
       <c r="B23" s="27"/>
       <c r="C23" s="25"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="24"/>
       <c r="B24" s="24"/>
       <c r="C24" s="25"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="24"/>
       <c r="B25" s="24"/>
       <c r="C25" s="25"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="24"/>
       <c r="B26" s="24"/>
       <c r="C26" s="25"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="24"/>
       <c r="B27" s="24"/>
       <c r="C27" s="25"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="24"/>
       <c r="B28" s="24"/>
       <c r="C28" s="25"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="24"/>
       <c r="B29" s="24"/>
       <c r="C29" s="25"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="24"/>
       <c r="B30" s="24"/>
       <c r="C30" s="25"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="24"/>
       <c r="B31" s="24"/>
       <c r="C31" s="25"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="24"/>
       <c r="B32" s="24"/>
       <c r="C32" s="25"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="24"/>
       <c r="B33" s="24"/>
       <c r="C33" s="25"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="24"/>
       <c r="B34" s="24"/>
       <c r="C34" s="25"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="25"/>
       <c r="B35" s="25"/>
       <c r="C35" s="26"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="25"/>
       <c r="B36" s="25"/>
       <c r="C36" s="26"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="25"/>
       <c r="B37" s="25"/>
       <c r="C37" s="26"/>
@@ -2624,24 +2623,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" style="3" customWidth="1"/>
-    <col min="6" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.265625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="42.1328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33.86328125" style="3" customWidth="1"/>
+    <col min="6" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="22" t="s">
         <v>6</v>
       </c>
@@ -2670,7 +2669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A2" s="21" t="s">
         <v>37</v>
       </c>
@@ -2687,7 +2686,7 @@
       <c r="H2" s="33"/>
       <c r="I2" s="33"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A3" s="21" t="s">
         <v>37</v>
       </c>
@@ -2706,7 +2705,7 @@
       <c r="H3" s="33"/>
       <c r="I3" s="33"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A4" s="21" t="s">
         <v>37</v>
       </c>
@@ -2725,7 +2724,7 @@
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A5" s="21" t="s">
         <v>37</v>
       </c>
@@ -2744,7 +2743,7 @@
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
     </row>
-    <row r="6" spans="1:10" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="35" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A6" s="21" t="s">
         <v>37</v>
       </c>
@@ -2763,7 +2762,7 @@
       <c r="H6" s="33"/>
       <c r="I6" s="33"/>
     </row>
-    <row r="7" spans="1:10" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="35" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A7" s="21" t="s">
         <v>37</v>
       </c>
@@ -2782,7 +2781,7 @@
       <c r="H7" s="33"/>
       <c r="I7" s="33"/>
     </row>
-    <row r="8" spans="1:10" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="35" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A8" s="21" t="s">
         <v>37</v>
       </c>
@@ -2803,7 +2802,7 @@
       </c>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:10" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="35" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A9" s="21" t="s">
         <v>37</v>
       </c>
@@ -2820,7 +2819,7 @@
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
       <c r="H9" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I9" s="33" t="s">
         <v>20</v>
@@ -2829,7 +2828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="35" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A10" s="21" t="s">
         <v>37</v>
       </c>
@@ -2848,7 +2847,7 @@
       <c r="H10" s="33"/>
       <c r="I10" s="33"/>
     </row>
-    <row r="11" spans="1:10" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="35" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A11" s="21" t="s">
         <v>37</v>
       </c>
@@ -2867,7 +2866,7 @@
       <c r="H11" s="33"/>
       <c r="I11" s="33"/>
     </row>
-    <row r="12" spans="1:10" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="35" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A12" s="21" t="s">
         <v>37</v>
       </c>
@@ -2890,7 +2889,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="35" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A13" s="21" t="s">
         <v>37</v>
       </c>
@@ -2909,7 +2908,7 @@
       <c r="H13" s="33"/>
       <c r="I13" s="33"/>
     </row>
-    <row r="14" spans="1:10" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="35" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A14" s="21" t="s">
         <v>37</v>
       </c>
@@ -2928,7 +2927,7 @@
       <c r="H14" s="33"/>
       <c r="I14" s="33"/>
     </row>
-    <row r="15" spans="1:10" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="35" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A15" s="21" t="s">
         <v>37</v>
       </c>
@@ -2954,7 +2953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="35" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A16" s="21" t="s">
         <v>37</v>
       </c>
@@ -2973,7 +2972,7 @@
       <c r="H16" s="54"/>
       <c r="I16" s="41"/>
     </row>
-    <row r="17" spans="1:10" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="35" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A17" s="21" t="s">
         <v>37</v>
       </c>
@@ -2999,7 +2998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="35" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A18" s="21" t="s">
         <v>37</v>
       </c>
@@ -3018,7 +3017,7 @@
       <c r="H18" s="54"/>
       <c r="I18" s="37"/>
     </row>
-    <row r="19" spans="1:10" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="20" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A19" s="21" t="s">
         <v>37</v>
       </c>
@@ -3037,7 +3036,7 @@
       <c r="H19" s="37"/>
       <c r="I19" s="37"/>
     </row>
-    <row r="20" spans="1:10" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="20" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A20" s="21" t="s">
         <v>37</v>
       </c>
@@ -3056,7 +3055,7 @@
       <c r="H20" s="37"/>
       <c r="I20" s="37"/>
     </row>
-    <row r="21" spans="1:10" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="20" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A21" s="21" t="s">
         <v>37</v>
       </c>
@@ -3075,7 +3074,7 @@
       <c r="H21" s="37"/>
       <c r="I21" s="37"/>
     </row>
-    <row r="22" spans="1:10" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="20" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A22" s="21" t="s">
         <v>37</v>
       </c>
@@ -3094,7 +3093,7 @@
       <c r="H22" s="37"/>
       <c r="I22" s="37"/>
     </row>
-    <row r="23" spans="1:10" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="20" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A23" s="21" t="s">
         <v>37</v>
       </c>
@@ -3120,7 +3119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="20" customFormat="1" ht="15.85" x14ac:dyDescent="0.45">
       <c r="A24" s="21" t="s">
         <v>37</v>
       </c>
@@ -3137,7 +3136,7 @@
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" spans="1:10" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="20" customFormat="1" ht="15.85" x14ac:dyDescent="0.45">
       <c r="A25" s="21" t="s">
         <v>37</v>
       </c>
@@ -3152,7 +3151,7 @@
       <c r="F25" s="42"/>
       <c r="G25" s="42"/>
       <c r="H25" s="42" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="I25" s="42" t="s">
         <v>20</v>
@@ -3161,7 +3160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="36" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A26" s="21" t="s">
         <v>37</v>
       </c>
@@ -3182,7 +3181,7 @@
       <c r="H26" s="42"/>
       <c r="I26" s="42"/>
     </row>
-    <row r="27" spans="1:10" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="36" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A27" s="21" t="s">
         <v>37</v>
       </c>
@@ -3208,7 +3207,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" s="36" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A28" s="21" t="s">
         <v>37</v>
       </c>
@@ -3229,7 +3228,7 @@
       <c r="H28" s="43"/>
       <c r="I28" s="43"/>
     </row>
-    <row r="29" spans="1:10" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="36" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A29" s="21" t="s">
         <v>37</v>
       </c>
@@ -3244,7 +3243,7 @@
       <c r="F29" s="43"/>
       <c r="G29" s="43"/>
       <c r="H29" s="43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I29" s="43" t="s">
         <v>20</v>
@@ -3253,7 +3252,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" s="36" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A30" s="21" t="s">
         <v>37</v>
       </c>
@@ -3268,7 +3267,7 @@
       <c r="F30" s="43"/>
       <c r="G30" s="43"/>
       <c r="H30" s="43" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I30" s="43" t="s">
         <v>20</v>
@@ -3277,7 +3276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" s="36" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A31" s="21" t="s">
         <v>37</v>
       </c>
@@ -3296,7 +3295,7 @@
       <c r="H31" s="43"/>
       <c r="I31" s="43"/>
     </row>
-    <row r="32" spans="1:10" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" s="36" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A32" s="21" t="s">
         <v>37</v>
       </c>
@@ -3313,7 +3312,7 @@
       <c r="F32" s="43"/>
       <c r="G32" s="43"/>
       <c r="H32" s="43" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="I32" s="43" t="s">
         <v>20</v>
@@ -3322,12 +3321,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="36" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A33" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B33" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="42" t="s">
         <v>24</v>
@@ -3339,16 +3338,16 @@
       <c r="H33" s="42"/>
       <c r="I33" s="42"/>
     </row>
-    <row r="34" spans="1:10" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" s="36" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A34" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="42"/>
       <c r="D34" s="51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>24</v>
@@ -3358,16 +3357,16 @@
       <c r="H34" s="52"/>
       <c r="I34" s="42"/>
     </row>
-    <row r="35" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.45">
       <c r="A35" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B35" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" s="42"/>
       <c r="D35" s="51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E35" s="42" t="s">
         <v>25</v>
@@ -3377,16 +3376,16 @@
       <c r="H35" s="42"/>
       <c r="I35" s="42"/>
     </row>
-    <row r="36" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.45">
       <c r="A36" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="42"/>
       <c r="D36" s="51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E36" s="42" t="s">
         <v>24</v>
@@ -3396,16 +3395,16 @@
       <c r="H36" s="42"/>
       <c r="I36" s="42"/>
     </row>
-    <row r="37" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.45">
       <c r="A37" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C37" s="42"/>
       <c r="D37" s="51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E37" s="42" t="s">
         <v>30</v>
@@ -3415,16 +3414,16 @@
       <c r="H37" s="42"/>
       <c r="I37" s="42"/>
     </row>
-    <row r="38" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.45">
       <c r="A38" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" s="42"/>
       <c r="D38" s="51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E38" s="42" t="s">
         <v>24</v>
@@ -3434,16 +3433,16 @@
       <c r="H38" s="42"/>
       <c r="I38" s="42"/>
     </row>
-    <row r="39" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.45">
       <c r="A39" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39" s="42"/>
       <c r="D39" s="51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E39" s="42" t="s">
         <v>26</v>
@@ -3451,7 +3450,7 @@
       <c r="F39" s="42"/>
       <c r="G39" s="42"/>
       <c r="H39" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I39" s="42" t="s">
         <v>20</v>
@@ -3460,16 +3459,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.45">
       <c r="A40" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B40" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" s="42"/>
       <c r="D40" s="42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E40" s="42" t="s">
         <v>24</v>
@@ -3479,16 +3478,16 @@
       <c r="H40" s="42"/>
       <c r="I40" s="42"/>
     </row>
-    <row r="41" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.45">
       <c r="A41" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B41" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C41" s="42"/>
       <c r="D41" s="42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E41" s="42" t="s">
         <v>25</v>
@@ -3498,12 +3497,12 @@
       <c r="H41" s="42"/>
       <c r="I41" s="42"/>
     </row>
-    <row r="42" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A42" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B42" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" s="42"/>
       <c r="D42" s="44" t="s">
@@ -3517,12 +3516,12 @@
       <c r="H42" s="42"/>
       <c r="I42" s="42"/>
     </row>
-    <row r="43" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A43" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B43" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43" s="42"/>
       <c r="D43" s="44" t="s">
@@ -3534,7 +3533,7 @@
       <c r="F43" s="42"/>
       <c r="G43" s="42"/>
       <c r="H43" s="42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I43" s="42" t="s">
         <v>20</v>
@@ -3543,16 +3542,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A44" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44" s="42"/>
       <c r="D44" s="44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E44" s="42" t="s">
         <v>24</v>
@@ -3562,16 +3561,16 @@
       <c r="H44" s="42"/>
       <c r="I44" s="42"/>
     </row>
-    <row r="45" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A45" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B45" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="42"/>
       <c r="D45" s="44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E45" s="42" t="s">
         <v>25</v>
@@ -3581,16 +3580,16 @@
       <c r="H45" s="42"/>
       <c r="I45" s="42"/>
     </row>
-    <row r="46" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A46" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B46" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C46" s="42"/>
       <c r="D46" s="44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E46" s="42" t="s">
         <v>24</v>
@@ -3600,12 +3599,12 @@
       <c r="H46" s="42"/>
       <c r="I46" s="42"/>
     </row>
-    <row r="47" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A47" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B47" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C47" s="42"/>
       <c r="D47" s="44" t="s">
@@ -3619,12 +3618,12 @@
       <c r="H47" s="52"/>
       <c r="I47" s="42"/>
     </row>
-    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A48" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B48" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" s="33"/>
       <c r="D48" s="44" t="s">
@@ -3636,7 +3635,7 @@
       <c r="F48" s="33"/>
       <c r="G48" s="33"/>
       <c r="H48" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I48" s="33" t="s">
         <v>20</v>
@@ -3645,12 +3644,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A49" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B49" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C49" s="33" t="s">
         <v>24</v>
@@ -3662,12 +3661,12 @@
       <c r="H49" s="33"/>
       <c r="I49" s="33"/>
     </row>
-    <row r="50" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A50" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B50" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C50" s="33" t="s">
         <v>30</v>
@@ -3679,12 +3678,12 @@
       <c r="H50" s="33"/>
       <c r="I50" s="33"/>
     </row>
-    <row r="51" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A51" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B51" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" s="33" t="s">
         <v>24</v>
@@ -3696,12 +3695,12 @@
       <c r="H51" s="33"/>
       <c r="I51" s="33"/>
     </row>
-    <row r="52" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A52" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B52" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C52" s="33" t="s">
         <v>25</v>
@@ -3713,12 +3712,12 @@
       <c r="H52" s="33"/>
       <c r="I52" s="33"/>
     </row>
-    <row r="53" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A53" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B53" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C53" s="33" t="s">
         <v>26</v>
@@ -3728,7 +3727,7 @@
       <c r="F53" s="33"/>
       <c r="G53" s="33"/>
       <c r="H53" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I53" s="33" t="s">
         <v>20</v>
@@ -3737,12 +3736,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A54" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B54" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54" s="33" t="s">
         <v>24</v>
@@ -3754,12 +3753,12 @@
       <c r="H54" s="33"/>
       <c r="I54" s="33"/>
     </row>
-    <row r="55" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A55" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B55" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C55" s="33" t="s">
         <v>26</v>
@@ -3769,7 +3768,7 @@
       <c r="F55" s="33"/>
       <c r="G55" s="33"/>
       <c r="H55" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I55" s="33" t="s">
         <v>20</v>
@@ -3778,12 +3777,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A56" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B56" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C56" s="33"/>
       <c r="D56" s="44" t="s">
@@ -3799,12 +3798,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A57" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B57" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" s="33"/>
       <c r="D57" s="44" t="s">
@@ -3816,7 +3815,7 @@
       <c r="F57" s="33"/>
       <c r="G57" s="33"/>
       <c r="H57" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I57" s="33" t="s">
         <v>20</v>
@@ -3825,7 +3824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" s="38" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A58" s="21" t="s">
         <v>37</v>
       </c>
@@ -3842,7 +3841,7 @@
       <c r="H58" s="33"/>
       <c r="I58" s="33"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="21" t="s">
         <v>37</v>
       </c>
@@ -3857,7 +3856,7 @@
       <c r="F59" s="16"/>
       <c r="G59" s="16"/>
       <c r="H59" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I59" s="16" t="s">
         <v>20</v>
@@ -3866,7 +3865,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="21" t="s">
         <v>37</v>
       </c>
@@ -3881,7 +3880,7 @@
       <c r="F60" s="16"/>
       <c r="G60" s="16"/>
       <c r="H60" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I60" s="16" t="s">
         <v>20</v>
@@ -3890,7 +3889,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" s="21" t="s">
         <v>37</v>
       </c>
@@ -3905,7 +3904,7 @@
       <c r="F61" s="16"/>
       <c r="G61" s="16"/>
       <c r="H61" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I61" s="16" t="s">
         <v>21</v>
@@ -3914,7 +3913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="21" t="s">
         <v>37</v>
       </c>
@@ -3929,7 +3928,7 @@
       <c r="F62" s="16"/>
       <c r="G62" s="16"/>
       <c r="H62" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I62" s="16" t="s">
         <v>21</v>
@@ -3938,7 +3937,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" s="21" t="s">
         <v>37</v>
       </c>
@@ -3962,7 +3961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" s="21" t="s">
         <v>37</v>
       </c>
@@ -3977,7 +3976,7 @@
       <c r="F64" s="16"/>
       <c r="G64" s="16"/>
       <c r="H64" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I64" s="16" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
08_01 recursos con directrices
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion02/EsqueletoGuion_CS_09_02_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion02/EsqueletoGuion_CS_09_02_CO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="80">
   <si>
     <t>FICHA</t>
   </si>
@@ -259,16 +259,13 @@
     <t>Autoevaluación</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: los felices años veinte</t>
-  </si>
-  <si>
     <t>Distingue las características del fascismo</t>
   </si>
   <si>
     <t>Cronología: el período de entreguerras</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje:  la Italia fascista</t>
+    <t>Los felices años 20</t>
   </si>
 </sst>
 </file>
@@ -1780,7 +1777,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E15" sqref="A15:E15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1912,7 +1909,7 @@
         <v>66</v>
       </c>
       <c r="D6" s="57" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="E6" s="57" t="s">
         <v>67</v>
@@ -1932,7 +1929,7 @@
         <v>66</v>
       </c>
       <c r="D7" s="59" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="E7" s="59" t="s">
         <v>67</v>
@@ -1972,7 +1969,7 @@
         <v>66</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E9" s="59" t="s">
         <v>67</v>
@@ -2096,7 +2093,7 @@
         <v>66</v>
       </c>
       <c r="D15" s="59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E15" s="59" t="s">
         <v>67</v>
@@ -2277,7 +2274,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2347,7 +2344,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>20</v>
@@ -2380,7 +2377,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>20</v>
@@ -2447,7 +2444,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>20</v>
@@ -2624,8 +2621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3152,7 +3149,7 @@
       <c r="F25" s="42"/>
       <c r="G25" s="42"/>
       <c r="H25" s="42" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="I25" s="42" t="s">
         <v>20</v>
@@ -3268,7 +3265,7 @@
       <c r="F30" s="43"/>
       <c r="G30" s="43"/>
       <c r="H30" s="43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I30" s="43" t="s">
         <v>20</v>
@@ -3313,7 +3310,7 @@
       <c r="F32" s="43"/>
       <c r="G32" s="43"/>
       <c r="H32" s="43" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="I32" s="43" t="s">
         <v>20</v>
@@ -3769,7 +3766,7 @@
       <c r="F55" s="33"/>
       <c r="G55" s="33"/>
       <c r="H55" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I55" s="33" t="s">
         <v>20</v>

</xml_diff>